<commit_message>
Small Correction Missings in Neutrality
</commit_message>
<xml_diff>
--- a/02_Raw_Data/Border_Data.xlsx
+++ b/02_Raw_Data/Border_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54c38c758baf9368/02_Studium/04_Econ_MSc/2-SS_2023/4423_Macroeconometrics/AdvMacroecotrics/Project/MacrometricsProject_2023/02_Raw_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fynn\Documents\GitHub\MacrometricsProject_2023\02_Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{356C768E-90D7-41EA-A607-25B4D2B78BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F999D129-A798-4BE8-9948-891AE6ECBDA6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22B2191-1187-4A1C-A1BA-7B1F484BF279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C550400C-416A-481C-8A3D-5A9277298504}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C550400C-416A-481C-8A3D-5A9277298504}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1071,18 +1071,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E077B94-7757-4643-9617-62A0F8C460A7}">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G148 G150:G175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.90625" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1124,8 +1124,11 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1144,8 +1147,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1164,8 +1170,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1184,8 +1193,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1204,8 +1216,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -1224,8 +1239,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1244,8 +1262,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -1264,8 +1285,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -1284,8 +1308,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -1304,8 +1331,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -1324,8 +1354,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -1344,8 +1377,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1364,8 +1400,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1384,8 +1423,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1404,8 +1446,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1424,8 +1469,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -1444,8 +1492,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1464,8 +1515,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1484,8 +1538,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -1504,8 +1561,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -1524,8 +1584,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1544,8 +1607,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1564,8 +1630,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -1584,8 +1653,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1604,8 +1676,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1624,8 +1699,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1644,8 +1722,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1664,8 +1745,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1684,8 +1768,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1704,8 +1791,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -1724,8 +1814,11 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1744,8 +1837,11 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>176</v>
       </c>
@@ -1764,8 +1860,11 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -1784,8 +1883,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1804,8 +1906,11 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1824,8 +1929,11 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -1844,8 +1952,11 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1864,8 +1975,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -1884,8 +1998,11 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -1904,8 +2021,11 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -1924,8 +2044,11 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>135</v>
       </c>
@@ -1944,8 +2067,11 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1964,8 +2090,11 @@
       <c r="F44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1984,8 +2113,11 @@
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -2004,8 +2136,11 @@
       <c r="F46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>154</v>
       </c>
@@ -2024,8 +2159,11 @@
       <c r="F47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2044,8 +2182,11 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2064,8 +2205,11 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -2084,8 +2228,11 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -2104,8 +2251,11 @@
       <c r="F51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2124,8 +2274,11 @@
       <c r="F52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2144,8 +2297,11 @@
       <c r="F53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>152</v>
       </c>
@@ -2164,8 +2320,11 @@
       <c r="F54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -2184,8 +2343,11 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -2204,8 +2366,11 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>137</v>
       </c>
@@ -2224,8 +2389,11 @@
       <c r="F57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2244,8 +2412,11 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>178</v>
       </c>
@@ -2264,8 +2435,11 @@
       <c r="F59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -2284,8 +2458,11 @@
       <c r="F60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -2304,8 +2481,11 @@
       <c r="F61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -2324,8 +2504,11 @@
       <c r="F62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -2344,8 +2527,11 @@
       <c r="F63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>139</v>
       </c>
@@ -2364,8 +2550,11 @@
       <c r="F64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>54</v>
       </c>
@@ -2384,8 +2573,11 @@
       <c r="F65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>21</v>
       </c>
@@ -2404,8 +2596,11 @@
       <c r="F66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -2424,8 +2619,11 @@
       <c r="F67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2444,8 +2642,11 @@
       <c r="F68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -2464,8 +2665,11 @@
       <c r="F69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -2484,8 +2688,11 @@
       <c r="F70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2504,8 +2711,11 @@
       <c r="F71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2524,8 +2734,11 @@
       <c r="F72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2544,8 +2757,11 @@
       <c r="F73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -2564,8 +2780,11 @@
       <c r="F74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -2584,8 +2803,11 @@
       <c r="F75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>156</v>
       </c>
@@ -2604,8 +2826,11 @@
       <c r="F76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -2624,8 +2849,11 @@
       <c r="F77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -2644,8 +2872,11 @@
       <c r="F78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>142</v>
       </c>
@@ -2664,8 +2895,11 @@
       <c r="F79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -2684,8 +2918,11 @@
       <c r="F80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -2704,8 +2941,11 @@
       <c r="F81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>158</v>
       </c>
@@ -2724,8 +2964,11 @@
       <c r="F82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -2744,8 +2987,11 @@
       <c r="F83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -2764,8 +3010,11 @@
       <c r="F84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>181</v>
       </c>
@@ -2784,8 +3033,11 @@
       <c r="F85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>180</v>
       </c>
@@ -2804,8 +3056,11 @@
       <c r="F86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>113</v>
       </c>
@@ -2824,8 +3079,11 @@
       <c r="F87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>159</v>
       </c>
@@ -2844,8 +3102,11 @@
       <c r="F88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>179</v>
       </c>
@@ -2864,8 +3125,11 @@
       <c r="F89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -2884,8 +3148,11 @@
       <c r="F90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -2904,8 +3171,11 @@
       <c r="F91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>160</v>
       </c>
@@ -2924,8 +3194,11 @@
       <c r="F92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -2944,8 +3217,11 @@
       <c r="F93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -2964,8 +3240,11 @@
       <c r="F94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -2984,8 +3263,11 @@
       <c r="F95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -3004,8 +3286,11 @@
       <c r="F96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -3024,8 +3309,11 @@
       <c r="F97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -3044,8 +3332,11 @@
       <c r="F98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>27</v>
       </c>
@@ -3064,8 +3355,11 @@
       <c r="F99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -3084,8 +3378,11 @@
       <c r="F100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>28</v>
       </c>
@@ -3104,8 +3401,11 @@
       <c r="F101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>144</v>
       </c>
@@ -3124,8 +3424,11 @@
       <c r="F102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>29</v>
       </c>
@@ -3144,8 +3447,11 @@
       <c r="F103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>30</v>
       </c>
@@ -3164,8 +3470,11 @@
       <c r="F104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>58</v>
       </c>
@@ -3184,8 +3493,11 @@
       <c r="F105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>128</v>
       </c>
@@ -3204,8 +3516,11 @@
       <c r="F106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>87</v>
       </c>
@@ -3224,8 +3539,11 @@
       <c r="F107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -3244,8 +3562,11 @@
       <c r="F108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -3264,8 +3585,11 @@
       <c r="F109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -3284,8 +3608,11 @@
       <c r="F110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>94</v>
       </c>
@@ -3304,8 +3631,11 @@
       <c r="F111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>32</v>
       </c>
@@ -3324,8 +3654,11 @@
       <c r="F112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>82</v>
       </c>
@@ -3344,8 +3677,11 @@
       <c r="F113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>145</v>
       </c>
@@ -3364,8 +3700,11 @@
       <c r="F114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>77</v>
       </c>
@@ -3384,8 +3723,11 @@
       <c r="F115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>59</v>
       </c>
@@ -3404,8 +3746,11 @@
       <c r="F116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -3424,8 +3769,11 @@
       <c r="F117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>34</v>
       </c>
@@ -3444,8 +3792,11 @@
       <c r="F118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -3464,8 +3815,11 @@
       <c r="F119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>146</v>
       </c>
@@ -3484,8 +3838,11 @@
       <c r="F120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>161</v>
       </c>
@@ -3504,8 +3861,11 @@
       <c r="F121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>83</v>
       </c>
@@ -3524,8 +3884,11 @@
       <c r="F122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>60</v>
       </c>
@@ -3544,8 +3907,11 @@
       <c r="F123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>78</v>
       </c>
@@ -3564,8 +3930,11 @@
       <c r="F124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>71</v>
       </c>
@@ -3584,8 +3953,11 @@
       <c r="F125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>72</v>
       </c>
@@ -3604,8 +3976,11 @@
       <c r="F126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>95</v>
       </c>
@@ -3624,8 +3999,11 @@
       <c r="F127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -3644,8 +4022,11 @@
       <c r="F128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>147</v>
       </c>
@@ -3664,8 +4045,11 @@
       <c r="F129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>162</v>
       </c>
@@ -3684,8 +4068,11 @@
       <c r="F130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>119</v>
       </c>
@@ -3704,8 +4091,11 @@
       <c r="F131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -3724,8 +4114,11 @@
       <c r="F132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>35</v>
       </c>
@@ -3744,8 +4137,11 @@
       <c r="F133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>163</v>
       </c>
@@ -3764,8 +4160,11 @@
       <c r="F134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>36</v>
       </c>
@@ -3784,8 +4183,11 @@
       <c r="F135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>120</v>
       </c>
@@ -3804,8 +4206,11 @@
       <c r="F136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>37</v>
       </c>
@@ -3824,8 +4229,11 @@
       <c r="F137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>38</v>
       </c>
@@ -3844,8 +4252,11 @@
       <c r="F138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>96</v>
       </c>
@@ -3864,8 +4275,11 @@
       <c r="F139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>121</v>
       </c>
@@ -3884,8 +4298,11 @@
       <c r="F140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>122</v>
       </c>
@@ -3904,8 +4321,11 @@
       <c r="F141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>39</v>
       </c>
@@ -3924,8 +4344,11 @@
       <c r="F142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>40</v>
       </c>
@@ -3944,8 +4367,11 @@
       <c r="F143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>41</v>
       </c>
@@ -3964,8 +4390,11 @@
       <c r="F144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>148</v>
       </c>
@@ -3984,8 +4413,11 @@
       <c r="F145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>84</v>
       </c>
@@ -4004,8 +4436,11 @@
       <c r="F146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -4024,8 +4459,11 @@
       <c r="F147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -4044,8 +4482,11 @@
       <c r="F148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>150</v>
       </c>
@@ -4068,7 +4509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -4087,8 +4528,11 @@
       <c r="F150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -4107,8 +4551,11 @@
       <c r="F151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>101</v>
       </c>
@@ -4127,8 +4574,11 @@
       <c r="F152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>44</v>
       </c>
@@ -4147,8 +4597,11 @@
       <c r="F153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>97</v>
       </c>
@@ -4167,8 +4620,11 @@
       <c r="F154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>98</v>
       </c>
@@ -4187,8 +4643,11 @@
       <c r="F155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>45</v>
       </c>
@@ -4207,8 +4666,11 @@
       <c r="F156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>61</v>
       </c>
@@ -4227,8 +4689,11 @@
       <c r="F157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>4</v>
       </c>
@@ -4247,8 +4712,11 @@
       <c r="F158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -4267,8 +4735,11 @@
       <c r="F159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>102</v>
       </c>
@@ -4287,8 +4758,11 @@
       <c r="F160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>46</v>
       </c>
@@ -4307,8 +4781,11 @@
       <c r="F161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>130</v>
       </c>
@@ -4327,8 +4804,11 @@
       <c r="F162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -4347,8 +4827,11 @@
       <c r="F163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>151</v>
       </c>
@@ -4367,8 +4850,11 @@
       <c r="F164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>63</v>
       </c>
@@ -4387,8 +4873,11 @@
       <c r="F165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>73</v>
       </c>
@@ -4407,8 +4896,11 @@
       <c r="F166">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>131</v>
       </c>
@@ -4427,8 +4919,11 @@
       <c r="F167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>103</v>
       </c>
@@ -4447,8 +4942,11 @@
       <c r="F168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>74</v>
       </c>
@@ -4467,8 +4965,11 @@
       <c r="F169">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>99</v>
       </c>
@@ -4487,8 +4988,11 @@
       <c r="F170">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>168</v>
       </c>
@@ -4507,8 +5011,11 @@
       <c r="F171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>167</v>
       </c>
@@ -4527,8 +5034,11 @@
       <c r="F172">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>123</v>
       </c>
@@ -4547,8 +5057,11 @@
       <c r="F173">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>47</v>
       </c>
@@ -4567,8 +5080,11 @@
       <c r="F174">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -4585,6 +5101,9 @@
         <v>0</v>
       </c>
       <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="G175">
         <v>0</v>
       </c>
     </row>
@@ -4604,7 +5123,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Plots and Analysis - Minor Changes with Data
</commit_message>
<xml_diff>
--- a/02_Raw_Data/Border_Data.xlsx
+++ b/02_Raw_Data/Border_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fynn\Documents\GitHub\MacrometricsProject_2023\02_Raw_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Paul\Documents\MacrometricsProject\MacrometricsProject_2023\02_Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22B2191-1187-4A1C-A1BA-7B1F484BF279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2245C8-A046-412C-81D6-2D88AA382D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C550400C-416A-481C-8A3D-5A9277298504}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C550400C-416A-481C-8A3D-5A9277298504}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -592,9 +592,6 @@
     <t>Syria</t>
   </si>
   <si>
-    <t>Türkiye</t>
-  </si>
-  <si>
     <t>United Arab Emirates</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
   </si>
   <si>
     <t>North Korea</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -1071,41 +1071,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E077B94-7757-4643-9617-62A0F8C460A7}">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G148 G150:G175"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="1" max="1" width="41.90625" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -1286,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1841,33 +1841,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>176</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>177</v>
-      </c>
       <c r="B35">
         <v>0</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>135</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>154</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>152</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>137</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2416,9 +2416,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -2439,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>139</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>54</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>21</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>156</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>142</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>158</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -3014,9 +3014,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -3037,9 +3037,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -3060,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>113</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>159</v>
       </c>
@@ -3106,9 +3106,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -3129,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>160</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>27</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>28</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>144</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>29</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>30</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>58</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>128</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>87</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>94</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>32</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>82</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>145</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>77</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>59</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>34</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>146</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>161</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>83</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>60</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>78</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>71</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>72</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>95</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>147</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>162</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>119</v>
       </c>
@@ -4095,15 +4095,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C132" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -4118,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>35</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>163</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>36</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>120</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>37</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>38</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>96</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>121</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>122</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>39</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>40</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>41</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>148</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>84</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>42</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>150</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>101</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>44</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>97</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>98</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>45</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>61</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>4</v>
       </c>
@@ -4716,9 +4716,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>102</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>46</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>130</v>
       </c>
@@ -4808,9 +4808,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -4831,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>151</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>63</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>73</v>
       </c>
@@ -4900,15 +4900,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>131</v>
       </c>
       <c r="B167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -4923,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>103</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>74</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>99</v>
       </c>
@@ -4992,9 +4992,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -5015,9 +5015,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -5038,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>123</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>47</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -5123,7 +5123,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>